<commit_message>
Updated GUI, /0 & /32 Subnet, Info Card
updated button
added error image
added info card (hover over image)
added /32 subnet
added /0 subnet
</commit_message>
<xml_diff>
--- a/Subnetting/Subnetting.xlsx
+++ b/Subnetting/Subnetting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\NetworkingTools\Subnetting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8743D0A9-29E0-4C93-9E0A-BA1B8D04C2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CE4024-2A2E-4B07-BB3A-941A57CA3E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="2130" windowWidth="20910" windowHeight="11835" activeTab="1" xr2:uid="{D396EB8A-540E-455F-90D8-37C94D7AED0E}"/>
+    <workbookView xWindow="4575" yWindow="5880" windowWidth="20910" windowHeight="11835" activeTab="1" xr2:uid="{D396EB8A-540E-455F-90D8-37C94D7AED0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Subnetting" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
   <si>
     <t>x</t>
   </si>
@@ -142,12 +142,18 @@
   </si>
   <si>
     <t>answers</t>
+  </si>
+  <si>
+    <t>informations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -246,24 +252,30 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,35 +611,35 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:26" x14ac:dyDescent="0.25">
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="P4" s="10" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="P4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
     </row>
     <row r="5" spans="4:26" x14ac:dyDescent="0.25">
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="1">
@@ -645,7 +657,7 @@
       <c r="I5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="13" t="s">
         <v>5</v>
       </c>
       <c r="Q5" s="1">
@@ -665,7 +677,7 @@
       </c>
     </row>
     <row r="6" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="9"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="1">
         <v>3</v>
       </c>
@@ -681,7 +693,7 @@
       <c r="I6" s="4">
         <v>0</v>
       </c>
-      <c r="P6" s="9"/>
+      <c r="P6" s="13"/>
       <c r="Q6" s="1">
         <v>3</v>
       </c>
@@ -699,7 +711,7 @@
       </c>
     </row>
     <row r="7" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="9"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="1">
         <v>2</v>
       </c>
@@ -715,7 +727,7 @@
       <c r="I7" s="4">
         <v>0</v>
       </c>
-      <c r="P7" s="9"/>
+      <c r="P7" s="13"/>
       <c r="Q7" s="1">
         <v>2</v>
       </c>
@@ -733,7 +745,7 @@
       </c>
     </row>
     <row r="8" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="9"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="1">
         <v>1</v>
       </c>
@@ -749,7 +761,7 @@
       <c r="I8" s="4">
         <v>0</v>
       </c>
-      <c r="P8" s="9"/>
+      <c r="P8" s="13"/>
       <c r="Q8" s="1">
         <v>1</v>
       </c>
@@ -767,7 +779,7 @@
       </c>
     </row>
     <row r="10" spans="4:26" x14ac:dyDescent="0.25">
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="1">
@@ -785,7 +797,7 @@
       <c r="I10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="P10" s="13" t="s">
         <v>6</v>
       </c>
       <c r="Q10" s="1">
@@ -805,7 +817,7 @@
       </c>
     </row>
     <row r="11" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="9"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="1">
         <v>3</v>
       </c>
@@ -821,7 +833,7 @@
       <c r="I11" s="4">
         <v>0</v>
       </c>
-      <c r="P11" s="9"/>
+      <c r="P11" s="13"/>
       <c r="Q11" s="1">
         <v>3</v>
       </c>
@@ -839,7 +851,7 @@
       </c>
     </row>
     <row r="12" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="9"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="1">
         <v>2</v>
       </c>
@@ -855,7 +867,7 @@
       <c r="I12" s="4">
         <v>0</v>
       </c>
-      <c r="P12" s="9"/>
+      <c r="P12" s="13"/>
       <c r="Q12" s="1">
         <v>2</v>
       </c>
@@ -873,7 +885,7 @@
       </c>
     </row>
     <row r="13" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="9"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="1">
         <v>1</v>
       </c>
@@ -889,7 +901,7 @@
       <c r="I13" s="4">
         <v>0</v>
       </c>
-      <c r="P13" s="9"/>
+      <c r="P13" s="13"/>
       <c r="Q13" s="1">
         <v>1</v>
       </c>
@@ -907,7 +919,7 @@
       </c>
     </row>
     <row r="15" spans="4:26" x14ac:dyDescent="0.25">
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="1">
@@ -925,7 +937,7 @@
       <c r="I15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="9" t="s">
+      <c r="P15" s="13" t="s">
         <v>7</v>
       </c>
       <c r="Q15" s="1">
@@ -945,7 +957,7 @@
       </c>
     </row>
     <row r="16" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="9"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="1">
         <v>3</v>
       </c>
@@ -961,7 +973,7 @@
       <c r="I16" s="4">
         <v>0</v>
       </c>
-      <c r="P16" s="9"/>
+      <c r="P16" s="13"/>
       <c r="Q16" s="1">
         <v>3</v>
       </c>
@@ -979,7 +991,7 @@
       </c>
     </row>
     <row r="17" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="9"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="1">
         <v>2</v>
       </c>
@@ -995,7 +1007,7 @@
       <c r="I17" s="4">
         <v>0</v>
       </c>
-      <c r="P17" s="9"/>
+      <c r="P17" s="13"/>
       <c r="Q17" s="1">
         <v>2</v>
       </c>
@@ -1013,7 +1025,7 @@
       </c>
     </row>
     <row r="18" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="9"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="1">
         <v>1</v>
       </c>
@@ -1029,19 +1041,19 @@
       <c r="I18" s="4">
         <v>0</v>
       </c>
-      <c r="P18" s="9"/>
+      <c r="P18" s="13"/>
       <c r="Q18" s="1">
         <v>1</v>
       </c>
-      <c r="R18" s="9" t="s">
+      <c r="R18" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
     </row>
     <row r="20" spans="4:31" x14ac:dyDescent="0.25">
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="13" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="1">
@@ -1059,7 +1071,7 @@
       <c r="I20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P20" s="9" t="s">
+      <c r="P20" s="13" t="s">
         <v>8</v>
       </c>
       <c r="Q20" s="1">
@@ -1079,7 +1091,7 @@
       </c>
     </row>
     <row r="21" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="9"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="1">
         <v>3</v>
       </c>
@@ -1095,7 +1107,7 @@
       <c r="I21" s="4">
         <v>255</v>
       </c>
-      <c r="P21" s="9"/>
+      <c r="P21" s="13"/>
       <c r="Q21" s="1">
         <v>3</v>
       </c>
@@ -1113,7 +1125,7 @@
       </c>
     </row>
     <row r="22" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="9"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="1">
         <v>2</v>
       </c>
@@ -1129,7 +1141,7 @@
       <c r="I22" s="4">
         <v>255</v>
       </c>
-      <c r="P22" s="9"/>
+      <c r="P22" s="13"/>
       <c r="Q22" s="1">
         <v>2</v>
       </c>
@@ -1147,7 +1159,7 @@
       </c>
     </row>
     <row r="23" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="9"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="1">
         <v>1</v>
       </c>
@@ -1163,7 +1175,7 @@
       <c r="I23" s="4">
         <v>255</v>
       </c>
-      <c r="P23" s="9"/>
+      <c r="P23" s="13"/>
       <c r="Q23" s="1">
         <v>1</v>
       </c>
@@ -1181,7 +1193,7 @@
       </c>
     </row>
     <row r="25" spans="4:31" x14ac:dyDescent="0.25">
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="1">
@@ -1214,7 +1226,7 @@
       <c r="N25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P25" s="9" t="s">
+      <c r="P25" s="13" t="s">
         <v>14</v>
       </c>
       <c r="Q25" s="1">
@@ -1249,7 +1261,7 @@
       </c>
     </row>
     <row r="26" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="9"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="1">
         <v>3</v>
       </c>
@@ -1280,7 +1292,7 @@
       <c r="N26" s="4">
         <v>254</v>
       </c>
-      <c r="P26" s="9"/>
+      <c r="P26" s="13"/>
       <c r="Q26" s="1">
         <v>3</v>
       </c>
@@ -1313,7 +1325,7 @@
       </c>
     </row>
     <row r="27" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="9"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="1">
         <v>2</v>
       </c>
@@ -1344,7 +1356,7 @@
       <c r="N27" s="4">
         <v>254</v>
       </c>
-      <c r="P27" s="9"/>
+      <c r="P27" s="13"/>
       <c r="Q27" s="1">
         <v>2</v>
       </c>
@@ -1377,7 +1389,7 @@
       </c>
     </row>
     <row r="28" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="9"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="1">
         <v>1</v>
       </c>
@@ -1408,7 +1420,7 @@
       <c r="N28" s="4">
         <v>254</v>
       </c>
-      <c r="P28" s="9"/>
+      <c r="P28" s="13"/>
       <c r="Q28" s="1">
         <v>1</v>
       </c>
@@ -1454,34 +1466,34 @@
       <c r="N30" s="5"/>
     </row>
     <row r="31" spans="4:31" x14ac:dyDescent="0.25">
-      <c r="D31" s="8">
+      <c r="D31" s="14">
         <v>4</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8">
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14">
         <v>3</v>
       </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8">
-        <v>2</v>
-      </c>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8">
-        <v>1</v>
-      </c>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14">
+        <v>2</v>
+      </c>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14">
+        <v>1</v>
+      </c>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
     </row>
     <row r="32" spans="4:31" x14ac:dyDescent="0.25">
       <c r="D32" s="6">
@@ -1837,40 +1849,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C198960-85DE-42F1-97C6-7B1974A6605C}">
-  <dimension ref="D3:F15"/>
+  <dimension ref="D3:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="P9" sqref="I1:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="13" t="s">
+    <row r="3" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="13" t="s">
+    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="8">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="14" t="s">
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>SUM(E3:E4)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="K5" s="8"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+    </row>
+    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>30</v>
       </c>
@@ -1881,7 +1907,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>31</v>
       </c>
@@ -1889,7 +1915,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>32</v>
       </c>
@@ -1897,7 +1923,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>33</v>
       </c>
@@ -1905,7 +1931,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>34</v>
       </c>
@@ -1913,27 +1939,37 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:13" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>35</v>
       </c>
       <c r="F14" s="12">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="16" t="s">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="12">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17">
-        <f>SUM(F9:F14)</f>
-        <v>0.99999999999999989</v>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17">
+        <f>SUM(F9:F15)</f>
+        <v>1.0049999999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D15:E15"/>
+  <mergeCells count="3">
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added User Option : Subnet Mask Address
* updated gui
* added subnet mask address user choice
* updated calculator
* fixed calculator / populateFields bugs
* added errors
* added comments
</commit_message>
<xml_diff>
--- a/Subnetting/Subnetting.xlsx
+++ b/Subnetting/Subnetting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\NetworkingTools\Subnetting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CE4024-2A2E-4B07-BB3A-941A57CA3E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14D5250-9E5C-4C8D-8141-2583F33407A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="5880" windowWidth="20910" windowHeight="11835" activeTab="1" xr2:uid="{D396EB8A-540E-455F-90D8-37C94D7AED0E}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{D396EB8A-540E-455F-90D8-37C94D7AED0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Subnetting" sheetId="4" r:id="rId1"/>
@@ -257,19 +257,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -611,35 +611,35 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:26" x14ac:dyDescent="0.25">
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="P4" s="15" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="P4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
     </row>
     <row r="5" spans="4:26" x14ac:dyDescent="0.25">
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="1">
@@ -657,7 +657,7 @@
       <c r="I5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="13" t="s">
+      <c r="P5" s="15" t="s">
         <v>5</v>
       </c>
       <c r="Q5" s="1">
@@ -677,7 +677,7 @@
       </c>
     </row>
     <row r="6" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="13"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="1">
         <v>3</v>
       </c>
@@ -693,7 +693,7 @@
       <c r="I6" s="4">
         <v>0</v>
       </c>
-      <c r="P6" s="13"/>
+      <c r="P6" s="15"/>
       <c r="Q6" s="1">
         <v>3</v>
       </c>
@@ -711,7 +711,7 @@
       </c>
     </row>
     <row r="7" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="13"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="1">
         <v>2</v>
       </c>
@@ -727,7 +727,7 @@
       <c r="I7" s="4">
         <v>0</v>
       </c>
-      <c r="P7" s="13"/>
+      <c r="P7" s="15"/>
       <c r="Q7" s="1">
         <v>2</v>
       </c>
@@ -745,7 +745,7 @@
       </c>
     </row>
     <row r="8" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="13"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="1">
         <v>1</v>
       </c>
@@ -761,7 +761,7 @@
       <c r="I8" s="4">
         <v>0</v>
       </c>
-      <c r="P8" s="13"/>
+      <c r="P8" s="15"/>
       <c r="Q8" s="1">
         <v>1</v>
       </c>
@@ -779,7 +779,7 @@
       </c>
     </row>
     <row r="10" spans="4:26" x14ac:dyDescent="0.25">
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="1">
@@ -797,7 +797,7 @@
       <c r="I10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P10" s="13" t="s">
+      <c r="P10" s="15" t="s">
         <v>6</v>
       </c>
       <c r="Q10" s="1">
@@ -817,7 +817,7 @@
       </c>
     </row>
     <row r="11" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="13"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="1">
         <v>3</v>
       </c>
@@ -833,7 +833,7 @@
       <c r="I11" s="4">
         <v>0</v>
       </c>
-      <c r="P11" s="13"/>
+      <c r="P11" s="15"/>
       <c r="Q11" s="1">
         <v>3</v>
       </c>
@@ -851,7 +851,7 @@
       </c>
     </row>
     <row r="12" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="13"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="1">
         <v>2</v>
       </c>
@@ -867,7 +867,7 @@
       <c r="I12" s="4">
         <v>0</v>
       </c>
-      <c r="P12" s="13"/>
+      <c r="P12" s="15"/>
       <c r="Q12" s="1">
         <v>2</v>
       </c>
@@ -885,7 +885,7 @@
       </c>
     </row>
     <row r="13" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="13"/>
+      <c r="D13" s="15"/>
       <c r="E13" s="1">
         <v>1</v>
       </c>
@@ -901,7 +901,7 @@
       <c r="I13" s="4">
         <v>0</v>
       </c>
-      <c r="P13" s="13"/>
+      <c r="P13" s="15"/>
       <c r="Q13" s="1">
         <v>1</v>
       </c>
@@ -919,7 +919,7 @@
       </c>
     </row>
     <row r="15" spans="4:26" x14ac:dyDescent="0.25">
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="1">
@@ -937,7 +937,7 @@
       <c r="I15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="13" t="s">
+      <c r="P15" s="15" t="s">
         <v>7</v>
       </c>
       <c r="Q15" s="1">
@@ -957,7 +957,7 @@
       </c>
     </row>
     <row r="16" spans="4:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="13"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="1">
         <v>3</v>
       </c>
@@ -973,7 +973,7 @@
       <c r="I16" s="4">
         <v>0</v>
       </c>
-      <c r="P16" s="13"/>
+      <c r="P16" s="15"/>
       <c r="Q16" s="1">
         <v>3</v>
       </c>
@@ -991,7 +991,7 @@
       </c>
     </row>
     <row r="17" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="13"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="1">
         <v>2</v>
       </c>
@@ -1007,7 +1007,7 @@
       <c r="I17" s="4">
         <v>0</v>
       </c>
-      <c r="P17" s="13"/>
+      <c r="P17" s="15"/>
       <c r="Q17" s="1">
         <v>2</v>
       </c>
@@ -1025,7 +1025,7 @@
       </c>
     </row>
     <row r="18" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="13"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="1">
         <v>1</v>
       </c>
@@ -1041,19 +1041,19 @@
       <c r="I18" s="4">
         <v>0</v>
       </c>
-      <c r="P18" s="13"/>
+      <c r="P18" s="15"/>
       <c r="Q18" s="1">
         <v>1</v>
       </c>
-      <c r="R18" s="13" t="s">
+      <c r="R18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
     </row>
     <row r="20" spans="4:31" x14ac:dyDescent="0.25">
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="1">
@@ -1071,7 +1071,7 @@
       <c r="I20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P20" s="13" t="s">
+      <c r="P20" s="15" t="s">
         <v>8</v>
       </c>
       <c r="Q20" s="1">
@@ -1091,7 +1091,7 @@
       </c>
     </row>
     <row r="21" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="13"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="1">
         <v>3</v>
       </c>
@@ -1107,7 +1107,7 @@
       <c r="I21" s="4">
         <v>255</v>
       </c>
-      <c r="P21" s="13"/>
+      <c r="P21" s="15"/>
       <c r="Q21" s="1">
         <v>3</v>
       </c>
@@ -1125,7 +1125,7 @@
       </c>
     </row>
     <row r="22" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="13"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="1">
         <v>2</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="I22" s="4">
         <v>255</v>
       </c>
-      <c r="P22" s="13"/>
+      <c r="P22" s="15"/>
       <c r="Q22" s="1">
         <v>2</v>
       </c>
@@ -1159,7 +1159,7 @@
       </c>
     </row>
     <row r="23" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="13"/>
+      <c r="D23" s="15"/>
       <c r="E23" s="1">
         <v>1</v>
       </c>
@@ -1175,7 +1175,7 @@
       <c r="I23" s="4">
         <v>255</v>
       </c>
-      <c r="P23" s="13"/>
+      <c r="P23" s="15"/>
       <c r="Q23" s="1">
         <v>1</v>
       </c>
@@ -1193,7 +1193,7 @@
       </c>
     </row>
     <row r="25" spans="4:31" x14ac:dyDescent="0.25">
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="1">
@@ -1226,7 +1226,7 @@
       <c r="N25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P25" s="13" t="s">
+      <c r="P25" s="15" t="s">
         <v>14</v>
       </c>
       <c r="Q25" s="1">
@@ -1261,7 +1261,7 @@
       </c>
     </row>
     <row r="26" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="13"/>
+      <c r="D26" s="15"/>
       <c r="E26" s="1">
         <v>3</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="N26" s="4">
         <v>254</v>
       </c>
-      <c r="P26" s="13"/>
+      <c r="P26" s="15"/>
       <c r="Q26" s="1">
         <v>3</v>
       </c>
@@ -1325,7 +1325,7 @@
       </c>
     </row>
     <row r="27" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="13"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="1">
         <v>2</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="N27" s="4">
         <v>254</v>
       </c>
-      <c r="P27" s="13"/>
+      <c r="P27" s="15"/>
       <c r="Q27" s="1">
         <v>2</v>
       </c>
@@ -1389,7 +1389,7 @@
       </c>
     </row>
     <row r="28" spans="4:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="13"/>
+      <c r="D28" s="15"/>
       <c r="E28" s="1">
         <v>1</v>
       </c>
@@ -1420,7 +1420,7 @@
       <c r="N28" s="4">
         <v>254</v>
       </c>
-      <c r="P28" s="13"/>
+      <c r="P28" s="15"/>
       <c r="Q28" s="1">
         <v>1</v>
       </c>
@@ -1466,34 +1466,34 @@
       <c r="N30" s="5"/>
     </row>
     <row r="31" spans="4:31" x14ac:dyDescent="0.25">
-      <c r="D31" s="14">
+      <c r="D31" s="16">
         <v>4</v>
       </c>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14">
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16">
         <v>3</v>
       </c>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14">
-        <v>2</v>
-      </c>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14">
-        <v>1</v>
-      </c>
-      <c r="T31" s="14"/>
-      <c r="U31" s="14"/>
-      <c r="V31" s="14"/>
-      <c r="W31" s="14"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16">
+        <v>2</v>
+      </c>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16">
+        <v>1</v>
+      </c>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="16"/>
     </row>
     <row r="32" spans="4:31" x14ac:dyDescent="0.25">
       <c r="D32" s="6">
@@ -1824,6 +1824,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P25:P28"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="I31:M31"/>
+    <mergeCell ref="N31:R31"/>
+    <mergeCell ref="S31:W31"/>
+    <mergeCell ref="D25:D28"/>
     <mergeCell ref="P4:Z4"/>
     <mergeCell ref="D5:D8"/>
     <mergeCell ref="D10:D13"/>
@@ -1835,12 +1841,6 @@
     <mergeCell ref="P10:P13"/>
     <mergeCell ref="P15:P18"/>
     <mergeCell ref="P20:P23"/>
-    <mergeCell ref="P25:P28"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="I31:M31"/>
-    <mergeCell ref="N31:R31"/>
-    <mergeCell ref="S31:W31"/>
-    <mergeCell ref="D25:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1852,7 +1852,7 @@
   <dimension ref="D3:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="I1:P9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1956,11 +1956,11 @@
       </c>
     </row>
     <row r="16" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17">
+      <c r="E16" s="17"/>
+      <c r="F16" s="13">
         <f>SUM(F9:F15)</f>
         <v>1.0049999999999999</v>
       </c>

</xml_diff>